<commit_message>
inserindo banco de dados
</commit_message>
<xml_diff>
--- a/resultados_avaliacao.xlsx
+++ b/resultados_avaliacao.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:N6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,30 +436,70 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>Tipo</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Nome</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Cargo</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Data</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>conquistas</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>desafios</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>autoavaliacao</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>objetivos</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
           <t>gestor</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>colaborador</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>pontos_fortes</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>areas_desenvolvimento</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>avaliacao</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>plano_desenvolvimento</t>
         </is>
@@ -468,33 +508,240 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>auto</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
           <t>iago</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>desenvolvedor full-stack</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>06/06/2025 14:56</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>aaaaaaaa</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>aaaaaaaaaa</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>aaaaaaaaaaaaaa</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr"/>
+      <c r="J2" t="inlineStr"/>
+      <c r="K2" t="inlineStr"/>
+      <c r="L2" t="inlineStr"/>
+      <c r="M2" t="inlineStr"/>
+      <c r="N2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>auto</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr"/>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>06/06/2025 18:00</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>iago</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
         <is>
           <t>Carlin</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Bom em design e edição de videos e fotos</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Design</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>aaaaaaaaaaaa</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>aaaaaaaaaaaaaa</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>aaaaaaaaaaaaaaaaaa</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>auto</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>ana</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>desenvolvedor full-stack</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>06/06/2025 22:18</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>aaaaa</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>aaaaaaaaaaa</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>aaaaaaaaaaaaaaaa</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr"/>
+      <c r="L4" t="inlineStr"/>
+      <c r="M4" t="inlineStr"/>
+      <c r="N4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>auto</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>gabi</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>design</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>06/06/2025 22:21</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>aaaa</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>aaaaaaaa</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
         <is>
           <t>5</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Colocar ele na área de design ou back-end
-</t>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>iago</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr"/>
+      <c r="J5" t="inlineStr"/>
+      <c r="K5" t="inlineStr"/>
+      <c r="L5" t="inlineStr"/>
+      <c r="M5" t="inlineStr"/>
+      <c r="N5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>auto</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr"/>
+      <c r="C6" t="inlineStr"/>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>06/06/2025 22:22</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="inlineStr"/>
+      <c r="H6" t="inlineStr"/>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>gabi</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>iago</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>teste</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>teste</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>teste 001</t>
         </is>
       </c>
     </row>

</xml_diff>